<commit_message>
Update project with IDF 4.4.2
</commit_message>
<xml_diff>
--- a/partitions/gen_partition/ESP32_Partition_Generator.xlsx
+++ b/partitions/gen_partition/ESP32_Partition_Generator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projetos\NOVUS\Telik-Smart-Trafo\Telik_Trafo_LTE\partitions\gen_partition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AF172C-8AB5-42B0-8460-A950213996A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A38FC9-10E2-41AF-BF96-F87F79FC6965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
@@ -134,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -206,8 +228,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +263,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,13 +310,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -305,8 +340,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bom" xfId="4" builtinId="26"/>
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,12 +560,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Planilha1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -594,15 +633,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <f>B5*(1024*1024)</f>
-        <v>1572864</v>
+        <v>1048576</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>180000</v>
+        <v>100000</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -614,9 +653,12 @@
       </c>
       <c r="B6">
         <f>(B4-B5)/2</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D6" s="4"/>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -624,19 +666,16 @@
       </c>
       <c r="B7">
         <f>(B4-B5)/2</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="I8" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -651,6 +690,10 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="I9" s="16" t="str" cm="1">
+        <f t="array" ref="I9">_xlfn.CONCAT(A9:E9&amp;", ", "Flags")</f>
+        <v># Name, Type, SubType, Offset, Size, Flags</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
@@ -678,6 +721,10 @@
       <c r="G10" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="I10" s="16" t="str">
+        <f>LOWER(_xlfn.CONCAT(A10,", ",B10,", ",C10,", 0x",D10,,", 0x",E10,", "))</f>
+        <v xml:space="preserve">nvs, data, nvs, 0x9000, 0x5000, </v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -704,6 +751,10 @@
       <c r="G11" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="I11" s="16" t="str">
+        <f>LOWER(_xlfn.CONCAT(A11,", ",B11,", ",C11,", 0x",D11,,", 0x",E11,", "))</f>
+        <v xml:space="preserve">otadata, data, ota, 0xe000, 0x2000, </v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -721,14 +772,18 @@
       </c>
       <c r="E12" s="1" t="str">
         <f>DEC2HEX((HEX2DEC(D4)-HEX2DEC(D5))/2)</f>
-        <v>140000</v>
+        <v>180000</v>
       </c>
       <c r="F12" s="10">
         <f>HEX2DEC(E12)/(1024*1024)</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>1</v>
+      </c>
+      <c r="I12" s="16" t="str">
+        <f t="shared" ref="I12:I14" si="2">LOWER(_xlfn.CONCAT(A12,", ",B12,", ",C12,", 0x",D12,,", 0x",E12,", "))</f>
+        <v xml:space="preserve">app0, app, ota_0, 0x10000, 0x180000, </v>
       </c>
       <c r="J12" s="8"/>
     </row>
@@ -744,18 +799,22 @@
       </c>
       <c r="D13" s="1" t="str">
         <f>DEC2HEX(HEX2DEC(D12) + HEX2DEC(E12))</f>
-        <v>150000</v>
+        <v>190000</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>DEC2HEX((HEX2DEC(D4)-HEX2DEC(D5))/2)</f>
-        <v>140000</v>
+        <v>180000</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" ref="F13:F14" si="2">HEX2DEC(E13)/(1024*1024)</f>
-        <v>1.25</v>
+        <f t="shared" ref="F13:F14" si="3">HEX2DEC(E13)/(1024*1024)</f>
+        <v>1.5</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>1</v>
+      </c>
+      <c r="I13" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">app1, app, ota_1, 0x190000, 0x180000, </v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
@@ -770,18 +829,22 @@
       </c>
       <c r="D14" s="1" t="str">
         <f>DEC2HEX(HEX2DEC(D13) + HEX2DEC(E13))</f>
-        <v>290000</v>
+        <v>310000</v>
       </c>
       <c r="E14" s="15" t="str">
         <f>DEC2HEX(C5-(64*1024))</f>
-        <v>170000</v>
+        <v>F0000</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="2"/>
-        <v>1.4375</v>
+        <f t="shared" si="3"/>
+        <v>0.9375</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>1</v>
+      </c>
+      <c r="I14" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">spiffs, data, spiffs, 0x310000, 0xf0000, </v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -825,11 +888,11 @@
         <v>14</v>
       </c>
       <c r="D19" s="9" t="str">
-        <f t="shared" ref="D19:E19" si="3">CONCATENATE("0x"&amp;D10)</f>
+        <f t="shared" ref="D19:E19" si="4">CONCATENATE("0x"&amp;D10)</f>
         <v>0x9000</v>
       </c>
       <c r="E19" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0x5000</v>
       </c>
       <c r="F19" s="9"/>
@@ -845,11 +908,11 @@
         <v>17</v>
       </c>
       <c r="D20" s="9" t="str">
-        <f t="shared" ref="D20:E20" si="4">CONCATENATE("0x"&amp;D11)</f>
+        <f t="shared" ref="D20:E20" si="5">CONCATENATE("0x"&amp;D11)</f>
         <v>0xE000</v>
       </c>
       <c r="E20" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0x2000</v>
       </c>
       <c r="F20" s="9"/>
@@ -869,8 +932,8 @@
         <v>0x10000</v>
       </c>
       <c r="E21" s="9" t="str">
-        <f t="shared" ref="E21" si="5">CONCATENATE("0x"&amp;E12)</f>
-        <v>0x140000</v>
+        <f t="shared" ref="E21" si="6">CONCATENATE("0x"&amp;E12)</f>
+        <v>0x180000</v>
       </c>
       <c r="F21" s="9"/>
     </row>
@@ -885,12 +948,12 @@
         <v>22</v>
       </c>
       <c r="D22" s="9" t="str">
-        <f t="shared" ref="D22:E22" si="6">CONCATENATE("0x"&amp;D13)</f>
-        <v>0x150000</v>
+        <f t="shared" ref="D22:E22" si="7">CONCATENATE("0x"&amp;D13)</f>
+        <v>0x190000</v>
       </c>
       <c r="E22" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>0x140000</v>
+        <f t="shared" si="7"/>
+        <v>0x180000</v>
       </c>
       <c r="F22" s="9"/>
     </row>
@@ -905,12 +968,12 @@
         <v>23</v>
       </c>
       <c r="D23" s="9" t="str">
-        <f t="shared" ref="D23:E23" si="7">CONCATENATE("0x"&amp;D14)</f>
-        <v>0x290000</v>
+        <f t="shared" ref="D23:E23" si="8">CONCATENATE("0x"&amp;D14)</f>
+        <v>0x310000</v>
       </c>
       <c r="E23" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>0x170000</v>
+        <f t="shared" si="8"/>
+        <v>0xF0000</v>
       </c>
       <c r="F23" s="9"/>
     </row>

</xml_diff>